<commit_message>
Updated Scrum Files on Sprint 2
</commit_message>
<xml_diff>
--- a/Project/Scrum board.xlsx
+++ b/Project/Scrum board.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafa\Desktop\SE2223_57514_60045_60602_60694_60700\Project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB1E608-69A9-43F9-A26A-79ECD3B38221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7migQJ+lrbl2DYfX+I5gs2U1BecDZA=="/>
@@ -16,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Backlog</t>
   </si>
@@ -83,36 +92,83 @@
   <si>
     <t>Pedro Lopes</t>
   </si>
+  <si>
+    <t>Collect a set of Metrics and explain their meaning (id 6)</t>
+  </si>
+  <si>
+    <t>Collect a set of Metrics and explain their meaning (id 7)</t>
+  </si>
+  <si>
+    <t>Collect a set of Metrics and explain their meaning (id 8)</t>
+  </si>
+  <si>
+    <t>Collect a set of Metrics and explain their meaning (id 9)</t>
+  </si>
+  <si>
+    <t>Collect a set of Metrics and explain their meaning (id 10)</t>
+  </si>
+  <si>
+    <t>Make 1 Use Case Diagram (id 11)</t>
+  </si>
+  <si>
+    <t>Make 1 Use Case Diagram (id 12)</t>
+  </si>
+  <si>
+    <t>Make 1 Use Case Diagram (id 13)</t>
+  </si>
+  <si>
+    <t>Make 1 Use Case Diagram (id 14)</t>
+  </si>
+  <si>
+    <t>Make 1 Use Case Diagram (id 15)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
-    <font/>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -150,211 +206,228 @@
         <bgColor rgb="FFFFE598"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFC9696"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor rgb="FFF7CAAC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
-    <border/>
+  <borders count="5">
     <border>
       <left/>
-      <top/>
-    </border>
-    <border>
       <right/>
       <top/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <top/>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+  <cellXfs count="40">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="8" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="12" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="14" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="14" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFC9696"/>
+    </mruColors>
+  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -544,195 +617,295 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:K1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="8.71"/>
-    <col customWidth="1" min="2" max="2" width="14.29"/>
-    <col customWidth="1" min="3" max="3" width="16.29"/>
-    <col customWidth="1" min="4" max="4" width="8.71"/>
-    <col customWidth="1" min="5" max="5" width="17.57"/>
-    <col customWidth="1" min="6" max="6" width="8.71"/>
-    <col customWidth="1" min="7" max="7" width="16.29"/>
-    <col customWidth="1" min="8" max="8" width="8.71"/>
-    <col customWidth="1" min="9" max="9" width="20.86"/>
-    <col customWidth="1" min="10" max="11" width="16.86"/>
-    <col customWidth="1" min="12" max="12" width="17.86"/>
-    <col customWidth="1" min="13" max="13" width="8.71"/>
-    <col customWidth="1" min="14" max="14" width="16.86"/>
-    <col customWidth="1" min="15" max="26" width="8.71"/>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" customWidth="1"/>
+    <col min="10" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" customWidth="1"/>
+    <col min="14" max="14" width="16.85546875" customWidth="1"/>
+    <col min="15" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1"/>
-    <row r="2" ht="14.25" customHeight="1">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="2:11" ht="14.25" customHeight="1">
+      <c r="D1" s="4"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+    </row>
+    <row r="2" spans="2:11" ht="14.25" customHeight="1">
+      <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="2" t="s">
+      <c r="E2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="2" t="s">
+      <c r="F2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="2" t="s">
+      <c r="G2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="3"/>
-      <c r="N2" s="1" t="s">
+      <c r="H2" s="5"/>
+      <c r="I2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="J2" s="5"/>
+      <c r="K2" s="6"/>
     </row>
-    <row r="3" ht="60.0" customHeight="1">
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="6"/>
-      <c r="J3" s="8" t="s">
+    <row r="3" spans="2:11" ht="60" customHeight="1">
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="9"/>
-      <c r="N3" s="10" t="s">
+      <c r="H3" s="29"/>
+      <c r="I3" s="24" t="s">
         <v>8</v>
       </c>
+      <c r="J3" s="8"/>
+      <c r="K3" s="6"/>
     </row>
-    <row r="4" ht="60.0" customHeight="1">
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="14" t="s">
+    <row r="4" spans="2:11" ht="60" customHeight="1">
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="17" t="s">
         <v>9</v>
       </c>
+      <c r="H4" s="29"/>
+      <c r="I4" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="8"/>
       <c r="K4" s="6"/>
-      <c r="N4" s="15" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="5" ht="60.0" customHeight="1">
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="18" t="s">
+    <row r="5" spans="2:11" ht="60" customHeight="1">
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="13"/>
-      <c r="N5" s="19" t="s">
+      <c r="H5" s="29"/>
+      <c r="I5" s="26" t="s">
         <v>12</v>
       </c>
+      <c r="J5" s="8"/>
+      <c r="K5" s="6"/>
     </row>
-    <row r="6" ht="60.0" customHeight="1">
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="13"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="20" t="s">
+    <row r="6" spans="2:11" ht="60" customHeight="1">
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="13"/>
-      <c r="N6" s="21" t="s">
+      <c r="H6" s="30"/>
+      <c r="I6" s="27" t="s">
         <v>14</v>
       </c>
+      <c r="J6" s="8"/>
+      <c r="K6" s="6"/>
     </row>
-    <row r="7" ht="60.0" customHeight="1">
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="26" t="s">
+    <row r="7" spans="2:11" ht="60" customHeight="1">
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="24"/>
-      <c r="N7" s="27" t="s">
+      <c r="H7" s="29"/>
+      <c r="I7" s="28" t="s">
         <v>16</v>
       </c>
+      <c r="J7" s="8"/>
+      <c r="K7" s="6"/>
     </row>
-    <row r="8" ht="60.0" customHeight="1">
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="30"/>
+    <row r="8" spans="2:11" ht="60" customHeight="1">
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="21"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="6"/>
     </row>
-    <row r="9" ht="60.0" customHeight="1">
-      <c r="D9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="J9" s="32"/>
+    <row r="9" spans="2:11" ht="60" customHeight="1">
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="19"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="39"/>
     </row>
-    <row r="10" ht="60.0" customHeight="1">
-      <c r="D10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="J10" s="32"/>
+    <row r="10" spans="2:11" ht="60" customHeight="1">
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="19"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="7"/>
     </row>
-    <row r="11" ht="60.0" customHeight="1">
-      <c r="D11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="J11" s="32"/>
+    <row r="11" spans="2:11" ht="60" customHeight="1">
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="19"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="7"/>
     </row>
-    <row r="12" ht="14.25" customHeight="1"/>
-    <row r="13" ht="14.25" customHeight="1"/>
-    <row r="14" ht="14.25" customHeight="1"/>
-    <row r="15" ht="14.25" customHeight="1"/>
-    <row r="16" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="12" spans="2:11" ht="60" customHeight="1">
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+    </row>
+    <row r="13" spans="2:11" ht="60" customHeight="1">
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="19"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+    </row>
+    <row r="14" spans="2:11" ht="60" customHeight="1">
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="19"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+    </row>
+    <row r="15" spans="2:11" ht="60" customHeight="1">
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="19"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+    </row>
+    <row r="16" spans="2:11" ht="60" customHeight="1">
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="19"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+    </row>
+    <row r="17" spans="2:9" ht="60" customHeight="1">
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="19"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+    </row>
+    <row r="18" spans="2:9" ht="60" customHeight="1"/>
+    <row r="19" spans="2:9" ht="60" customHeight="1"/>
+    <row r="20" spans="2:9" ht="60" customHeight="1"/>
+    <row r="21" spans="2:9" ht="60" customHeight="1"/>
+    <row r="22" spans="2:9" ht="60" customHeight="1"/>
+    <row r="23" spans="2:9" ht="60" customHeight="1"/>
+    <row r="24" spans="2:9" ht="14.25" customHeight="1"/>
+    <row r="25" spans="2:9" ht="14.25" customHeight="1"/>
+    <row r="26" spans="2:9" ht="14.25" customHeight="1"/>
+    <row r="27" spans="2:9" ht="14.25" customHeight="1"/>
+    <row r="28" spans="2:9" ht="14.25" customHeight="1"/>
+    <row r="29" spans="2:9" ht="14.25" customHeight="1"/>
+    <row r="30" spans="2:9" ht="14.25" customHeight="1"/>
+    <row r="31" spans="2:9" ht="14.25" customHeight="1"/>
+    <row r="32" spans="2:9" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1702,51 +1875,7 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <mergeCells count="40">
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="J5:K5"/>
-  </mergeCells>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>